<commit_message>
Added local errors, fixed test cases
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>LastReportTimeAssetName</t>
+  </si>
+  <si>
+    <t>ErrorCodePath</t>
+  </si>
+  <si>
+    <t>Data\ErrorCodes.xlsx</t>
   </si>
 </sst>
 </file>
@@ -875,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1157,22 +1163,29 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Actualizado con nueva librería de Mail
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -298,27 +298,12 @@
     <t>MailProcessFullName</t>
   </si>
   <si>
-    <t>MailProcessShortName</t>
-  </si>
-  <si>
-    <t>MailProcessNickName</t>
-  </si>
-  <si>
-    <t>PRN</t>
-  </si>
-  <si>
     <t>MailSenderName</t>
   </si>
   <si>
     <t>Name that will be sent on emails</t>
   </si>
   <si>
-    <t>MailCountry</t>
-  </si>
-  <si>
-    <t>España</t>
-  </si>
-  <si>
     <t>ConstantesEnvioMail</t>
   </si>
   <si>
@@ -335,9 +320,6 @@
   </si>
   <si>
     <t>ProcessModule</t>
-  </si>
-  <si>
-    <t>Colector/Consumidor</t>
   </si>
   <si>
     <t>MailContactLanguage</t>
@@ -481,6 +463,33 @@
   </si>
   <si>
     <t>Data\ErrorCodes.xlsx</t>
+  </si>
+  <si>
+    <t>TemplateReport</t>
+  </si>
+  <si>
+    <t>Data\Template_Report.xlsx</t>
+  </si>
+  <si>
+    <t>ReportName</t>
+  </si>
+  <si>
+    <t>SheetDetails</t>
+  </si>
+  <si>
+    <t>Detalle</t>
+  </si>
+  <si>
+    <t>SheetSummary</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Reporter</t>
+  </si>
+  <si>
+    <t>Reportname_{0}.xlsx</t>
   </si>
 </sst>
 </file>
@@ -879,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1012"/>
+  <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -940,22 +949,22 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="45">
@@ -967,215 +976,251 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="30">
-      <c r="A7" t="s">
+    <row r="6" spans="1:26">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="30">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>129</v>
-      </c>
+    <row r="13" spans="1:26">
+      <c r="B13" s="2"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C16" s="4"/>
+      <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C17" s="4"/>
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="8" t="s">
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B26" s="8"/>
+      <c r="B26" s="8" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
         <v>102</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="B28" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B29" t="s">
-        <v>105</v>
+      <c r="B29" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>113</v>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>105</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B31" s="8"/>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>143</v>
-      </c>
-      <c r="B33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2150,6 +2195,11 @@
     <row r="1010" ht="14.25" customHeight="1"/>
     <row r="1011" ht="14.25" customHeight="1"/>
     <row r="1012" ht="14.25" customHeight="1"/>
+    <row r="1013" ht="14.25" customHeight="1"/>
+    <row r="1014" ht="14.25" customHeight="1"/>
+    <row r="1015" ht="14.25" customHeight="1"/>
+    <row r="1016" ht="14.25" customHeight="1"/>
+    <row r="1017" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2159,10 +2209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z951"/>
+  <dimension ref="A1:Z948"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2346,10 +2396,10 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -2475,10 +2525,10 @@
     </row>
     <row r="35" spans="1:3" s="6" customFormat="1" ht="14.25" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
@@ -2486,7 +2536,7 @@
         <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
         <v>88</v>
@@ -2497,50 +2547,23 @@
         <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" t="s">
-        <v>124</v>
-      </c>
-      <c r="C39" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" t="s">
-        <v>99</v>
-      </c>
-    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3448,9 +3471,6 @@
     <row r="946" ht="14.25" customHeight="1"/>
     <row r="947" ht="14.25" customHeight="1"/>
     <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3463,7 +3483,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3515,7 +3535,7 @@
         <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -3529,7 +3549,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -3540,7 +3560,7 @@
         <v>54</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
         <v>60</v>
@@ -3548,13 +3568,13 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4614,7 +4634,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -5660,7 +5680,7 @@
         <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -5690,12 +5710,12 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="D2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1">
       <c r="D3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Quitado continueonerror, añadido MailBody en config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -478,6 +478,15 @@
   </si>
   <si>
     <t>NoReplyMail</t>
+  </si>
+  <si>
+    <t>MailBody</t>
+  </si>
+  <si>
+    <t>Modify as required</t>
+  </si>
+  <si>
+    <t>Adjuntamos reporte de ejecución</t>
   </si>
 </sst>
 </file>
@@ -876,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1017"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1165,51 +1174,61 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B31" s="8"/>
+      <c r="A31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
+      <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
         <v>94</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
-    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
         <v>104</v>
       </c>
-      <c r="B35" t="b">
+      <c r="B36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" t="s">
-        <v>129</v>
-      </c>
-    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
         <v>132</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2188,6 +2207,7 @@
     <row r="1015" ht="14.25" customHeight="1"/>
     <row r="1016" ht="14.25" customHeight="1"/>
     <row r="1017" ht="14.25" customHeight="1"/>
+    <row r="1018" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>